<commit_message>
Modification masque de saisie
</commit_message>
<xml_diff>
--- a/metadata/Masque de saisie.xlsx
+++ b/metadata/Masque de saisie.xlsx
@@ -22,94 +22,94 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>numrodeligne</t>
-  </si>
-  <si>
-    <t>dataentryby</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>sheet</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>Exportsimports</t>
-  </si>
-  <si>
-    <t>marchandises</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
-    <t>pays</t>
-  </si>
-  <si>
-    <t>quantit</t>
-  </si>
-  <si>
-    <t>Unité de poids/quantité</t>
-  </si>
-  <si>
-    <t>Prix unitaire / unité de compte Lt</t>
-  </si>
-  <si>
-    <t>Prix unitaire / unité de compte Sous</t>
-  </si>
-  <si>
-    <t>Prix unitaire / unité de compte Deniers</t>
-  </si>
-  <si>
-    <t>Prix unitaire en  Lt (décimale)</t>
-  </si>
-  <si>
-    <t>Valeur / unité de compte Lt</t>
-  </si>
-  <si>
-    <t>Valeur / unité de compte Sous</t>
-  </si>
-  <si>
-    <t>Valeur/ unité de compte Deniers</t>
-  </si>
-  <si>
-    <t>Valeur en décimales de livres tournois</t>
-  </si>
-  <si>
-    <t>Valeur en décimales de livres tournois (multipliée)</t>
-  </si>
-  <si>
-    <t>problem</t>
-  </si>
-  <si>
-    <t>remarks</t>
-  </si>
-  <si>
-    <t>doubleaccount</t>
-  </si>
-  <si>
-    <t>Hasna</t>
-  </si>
-  <si>
-    <t>CCI Marseille - I 30</t>
-  </si>
-  <si>
-    <t>Import</t>
-  </si>
-  <si>
-    <t>bierre</t>
-  </si>
-  <si>
-    <t>Marseille</t>
-  </si>
-  <si>
-    <t>Angleterre</t>
-  </si>
-  <si>
-    <t>livres</t>
+    <t xml:space="preserve">numrodeligne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataentryby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportsimports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marchandises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unité de poids/quantité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix unitaire / unité de compte Lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix unitaire / unité de compte Sous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix unitaire / unité de compte Deniers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix unitaire en  Lt (décimale)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur / unité de compte Lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur / unité de compte Sous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur/ unité de compte Deniers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur en décimales de livres tournois dans la source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur en décimales de livres tournois (multipliée)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doubleaccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCI Marseille - I 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marseille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angleterre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">livres</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="@"/>
@@ -400,33 +400,33 @@
   </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.11737089201878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.981220657277"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.11737089201878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.43661971830986"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5399061032864"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6291079812207"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.5399061032864"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5774647887324"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.5492957746479"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9530516431925"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.4976525821596"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.5399061032864"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.76056338028169"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="15.7323943661972"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2159624413146"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="10.5399061032864"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5492957746479"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3615023474178"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.6009389671362"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="23.3615023474178"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.5399061032864"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.18779342723005"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3051643192488"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.18779342723005"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.51173708920188"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6338028169014"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1173708920188"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6338028169014"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8169014084507"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7887323943662"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.2018779342723"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.7370892018779"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6338028169014"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.84507042253521"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="15.981220657277"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.4647887323944"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="10.6338028169014"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.7887323943662"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.6009389671362"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.849765258216"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="23.7652582159624"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.6338028169014"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="65.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Dieppe en excel et réorganisation
Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/metadata/Masque de saisie.xlsx
+++ b/metadata/Masque de saisie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/toflit18_data_GIT/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E9961-8E5B-814F-8BA0-DA4602BB1F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB3F49-3E1B-8048-AC56-5C28B983A8C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25020" windowHeight="15260" tabRatio="984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>source</t>
   </si>
@@ -77,9 +77,6 @@
     <t>width_in_line</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>value_part_of_bundle</t>
   </si>
   <si>
@@ -143,49 +140,49 @@
     <t>duty_remarks</t>
   </si>
   <si>
-    <t>Rouen</t>
-  </si>
-  <si>
-    <t>Le Havre</t>
-  </si>
-  <si>
-    <t>les4villesansatiques</t>
-  </si>
-  <si>
-    <t>Exports</t>
-  </si>
-  <si>
-    <t>Arbres ; fruitiers</t>
-  </si>
-  <si>
-    <t>sources/National toutes directions partenaires manquants/AN_F12_1666_Rouen_Exports_1789.csv</t>
-  </si>
-  <si>
-    <t>AN F12 1666</t>
-  </si>
-  <si>
-    <t>Jérémy Hervelin</t>
-  </si>
-  <si>
-    <t>angleterre</t>
-  </si>
-  <si>
-    <t>Bêtes ; de somme ; chevaux</t>
-  </si>
-  <si>
-    <t>en nombre</t>
-  </si>
-  <si>
-    <t>marseilles</t>
-  </si>
-  <si>
-    <t>Beurre ; salé</t>
-  </si>
-  <si>
-    <t>Normandie</t>
-  </si>
-  <si>
-    <t>espagne</t>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>value (annoncée)</t>
+  </si>
+  <si>
+    <t>Balais de palme</t>
+  </si>
+  <si>
+    <t>value (calculée)</t>
+  </si>
+  <si>
+    <t>douzaine</t>
+  </si>
+  <si>
+    <t>Guillaume Daudin</t>
+  </si>
+  <si>
+    <t>Archives de la CCI de Marseille - I 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local/Marseille/Archives_de_la_CCI_de_Marseille-I32/Marseille – Imports – 1749.csv	</t>
+  </si>
+  <si>
+    <t>Bœuf salé</t>
+  </si>
+  <si>
+    <t>Bierre</t>
+  </si>
+  <si>
+    <t>Bled froment</t>
+  </si>
+  <si>
+    <t>Bois à brûler</t>
+  </si>
+  <si>
+    <t>charges</t>
   </si>
 </sst>
 </file>
@@ -196,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -208,6 +205,18 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,11 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -631,20 +641,20 @@
     <col min="9" max="9" width="26.1640625"/>
     <col min="10" max="10" width="15.83203125"/>
     <col min="11" max="11" width="13.83203125"/>
-    <col min="12" max="12" width="17.1640625"/>
-    <col min="13" max="13" width="12.6640625" style="1"/>
-    <col min="14" max="14" width="10.6640625"/>
-    <col min="16" max="16" width="16" style="2"/>
-    <col min="17" max="17" width="13.5"/>
-    <col min="18" max="19" width="10.6640625"/>
-    <col min="20" max="20" width="13.83203125"/>
-    <col min="21" max="21" width="14.6640625"/>
-    <col min="22" max="22" width="14.83203125"/>
-    <col min="23" max="23" width="23.83203125"/>
-    <col min="24" max="1026" width="10.6640625"/>
+    <col min="13" max="13" width="17.1640625"/>
+    <col min="14" max="14" width="12.6640625" style="1"/>
+    <col min="15" max="15" width="10.6640625"/>
+    <col min="17" max="17" width="16" style="2"/>
+    <col min="18" max="18" width="13.5"/>
+    <col min="19" max="20" width="10.6640625"/>
+    <col min="21" max="21" width="13.83203125"/>
+    <col min="22" max="22" width="14.6640625"/>
+    <col min="23" max="23" width="14.83203125"/>
+    <col min="24" max="24" width="23.83203125"/>
+    <col min="25" max="1027" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -676,137 +686,149 @@
         <v>13</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="3" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C2" s="3">
-        <v>1789</v>
+        <v>1749</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="L2" s="3">
+        <f>N2*P2</f>
+        <v>22.5</v>
+      </c>
+      <c r="M2" s="3">
         <v>0</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
+      <c r="N2" s="3">
+        <v>25</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="P2" s="3">
+        <f>18/20</f>
+        <v>0.9</v>
+      </c>
       <c r="Q2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="3">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="S2" s="3">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
+      <c r="AA2" s="3">
+        <f>K2-L2</f>
+        <v>-0.5</v>
+      </c>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
@@ -815,63 +837,74 @@
       <c r="AG2" s="3"/>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C3" s="3">
-        <v>1789</v>
+        <v>1749</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3">
-        <v>117</v>
+        <f>11795</f>
+        <v>11795</v>
       </c>
       <c r="L3" s="3">
+        <f t="shared" ref="L3:L6" si="0">N3*P3</f>
+        <v>11795</v>
+      </c>
+      <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3" t="s">
-        <v>41</v>
+      <c r="N3" s="3">
+        <v>33700</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <f>7/20</f>
+        <v>0.35</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="3">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="S3" s="3">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
-      <c r="W3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
+      <c r="AA3" s="3">
+        <f t="shared" ref="AA3:AA6" si="1">K3-L3</f>
+        <v>0</v>
+      </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
@@ -880,67 +913,73 @@
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C4" s="3">
-        <v>1789</v>
+        <v>1749</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3">
-        <v>600</v>
+        <v>75</v>
       </c>
       <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="M4" s="3">
         <v>0</v>
       </c>
-      <c r="M4" s="3">
-        <v>2</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
-        <v>41</v>
+      <c r="N4" s="3">
+        <v>1500</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="3">
+        <f>1/20</f>
+        <v>0.05</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" s="3">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="S4" s="3">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
+      <c r="AA4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
@@ -949,69 +988,72 @@
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C5" s="3">
-        <v>1789</v>
+        <v>1749</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3">
-        <v>160</v>
+        <v>9242650</v>
       </c>
       <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>9242650</v>
+      </c>
+      <c r="M5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="3">
-        <v>100</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3" t="s">
-        <v>41</v>
+      <c r="N5" s="3">
+        <v>369706</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="3">
+        <v>25</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5" s="3">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="S5" s="3">
-        <v>1080</v>
+        <v>1</v>
       </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+      <c r="AA5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
@@ -1020,69 +1062,73 @@
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C6" s="3">
-        <v>1789</v>
+        <v>1749</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3">
-        <v>1080</v>
+        <v>270</v>
       </c>
       <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>270.00000000000006</v>
+      </c>
+      <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="M6" s="3">
-        <v>1350</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="3">
+        <v>30000</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3" t="s">
-        <v>41</v>
+      <c r="P6" s="3">
+        <f>18/20/100</f>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="3">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="S6" s="3">
-        <v>1080</v>
+        <v>1</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+      <c r="AA6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
@@ -1091,8 +1137,10 @@
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>